<commit_message>
Update HH member absent return date prompt
</commit_message>
<xml_diff>
--- a/odkx/app/config/tables/hh_member/forms/hh_member_new/hh_member_new.xlsx
+++ b/odkx/app/config/tables/hh_member/forms/hh_member_new/hh_member_new.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1663" uniqueCount="619">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1661" uniqueCount="617">
   <si>
     <t xml:space="preserve">clause</t>
   </si>
@@ -968,6 +968,9 @@
     <t xml:space="preserve">tomorrow</t>
   </si>
   <si>
+    <t xml:space="preserve">date</t>
+  </si>
+  <si>
     <t xml:space="preserve">time_awake</t>
   </si>
   <si>
@@ -1595,16 +1598,7 @@
     <t xml:space="preserve">absent_return_date</t>
   </si>
   <si>
-    <t xml:space="preserve">date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">absent_return_integer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">absent_return_dwmy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">absent_return_dk</t>
+    <t xml:space="preserve">date_no_time</t>
   </si>
   <si>
     <t xml:space="preserve">Member Left</t>
@@ -2253,9 +2247,9 @@
   <dimension ref="A1:T92"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F86" activeCellId="0" sqref="F86"/>
+      <selection pane="bottomLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.25" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4346,10 +4340,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C400"/>
+  <dimension ref="A1:C402"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A169" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A205" activeCellId="0" sqref="A205"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A169" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A209" activeCellId="0" sqref="A209"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.25" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6649,156 +6643,156 @@
     </row>
     <row r="209" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="0" t="s">
+        <v>311</v>
+      </c>
+      <c r="B209" s="0" t="s">
         <v>314</v>
       </c>
-      <c r="B209" s="0" t="s">
-        <v>315</v>
-      </c>
       <c r="C209" s="0" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="0" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="B210" s="0" t="s">
-        <v>316</v>
+        <v>58</v>
       </c>
       <c r="C210" s="0" t="s">
-        <v>316</v>
+        <v>58</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="0" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B211" s="0" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C211" s="0" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="0" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B212" s="0" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C212" s="0" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="0" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="B213" s="0" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C213" s="0" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="0" t="s">
+        <v>315</v>
+      </c>
+      <c r="B214" s="0" t="s">
         <v>319</v>
       </c>
-      <c r="B214" s="0" t="s">
-        <v>321</v>
-      </c>
       <c r="C214" s="0" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="0" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B215" s="0" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C215" s="0" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="0" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B216" s="0" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C216" s="0" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="0" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B217" s="0" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C217" s="0" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="0" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="B218" s="0" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="C218" s="0" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="0" t="s">
+        <v>320</v>
+      </c>
+      <c r="B219" s="0" t="s">
         <v>325</v>
       </c>
-      <c r="B219" s="0" t="s">
-        <v>321</v>
-      </c>
       <c r="C219" s="0" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="0" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B220" s="0" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C220" s="0" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="0" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B221" s="0" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C221" s="0" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="0" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B222" s="0" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C222" s="0" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6806,10 +6800,10 @@
         <v>326</v>
       </c>
       <c r="B223" s="0" t="s">
-        <v>315</v>
+        <v>324</v>
       </c>
       <c r="C223" s="0" t="s">
-        <v>315</v>
+        <v>324</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6817,32 +6811,32 @@
         <v>326</v>
       </c>
       <c r="B224" s="0" t="s">
-        <v>316</v>
+        <v>325</v>
       </c>
       <c r="C224" s="0" t="s">
-        <v>316</v>
+        <v>325</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="0" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B225" s="0" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C225" s="0" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="0" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B226" s="0" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C226" s="0" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6850,10 +6844,10 @@
         <v>327</v>
       </c>
       <c r="B227" s="0" t="s">
-        <v>328</v>
+        <v>318</v>
       </c>
       <c r="C227" s="0" t="s">
-        <v>328</v>
+        <v>318</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6861,329 +6855,329 @@
         <v>327</v>
       </c>
       <c r="B228" s="0" t="s">
-        <v>329</v>
+        <v>319</v>
       </c>
       <c r="C228" s="0" t="s">
-        <v>329</v>
+        <v>319</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="0" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B229" s="0" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C229" s="0" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="0" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B230" s="0" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C230" s="0" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="0" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B231" s="0" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C231" s="0" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="0" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B232" s="0" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C232" s="0" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="0" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B233" s="0" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C233" s="0" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="0" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B234" s="0" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C234" s="0" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="0" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B235" s="0" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C235" s="0" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A236" s="0" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B236" s="0" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C236" s="0" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="0" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B237" s="0" t="s">
-        <v>204</v>
+        <v>337</v>
       </c>
       <c r="C237" s="0" t="s">
-        <v>204</v>
+        <v>337</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="0" t="s">
+        <v>328</v>
+      </c>
+      <c r="B238" s="0" t="s">
         <v>338</v>
       </c>
-      <c r="B238" s="0" t="s">
-        <v>339</v>
-      </c>
       <c r="C238" s="0" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="0" t="s">
-        <v>338</v>
+        <v>328</v>
       </c>
       <c r="B239" s="0" t="s">
-        <v>340</v>
+        <v>204</v>
       </c>
       <c r="C239" s="0" t="s">
-        <v>340</v>
+        <v>204</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="0" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B240" s="0" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C240" s="0" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="0" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B241" s="0" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C241" s="0" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="0" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B242" s="0" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C242" s="0" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="0" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B243" s="0" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C243" s="0" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="0" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B244" s="0" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C244" s="0" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="0" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B245" s="0" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C245" s="0" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="246" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="0" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B246" s="0" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C246" s="0" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="247" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="0" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B247" s="0" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C247" s="0" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="248" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="0" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B248" s="0" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C248" s="0" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="249" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="0" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B249" s="0" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C249" s="0" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="250" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A250" s="0" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B250" s="0" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C250" s="0" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="251" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A251" s="0" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B251" s="0" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C251" s="0" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="252" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A252" s="0" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B252" s="0" t="s">
-        <v>58</v>
+        <v>352</v>
       </c>
       <c r="C252" s="0" t="s">
-        <v>58</v>
+        <v>352</v>
       </c>
     </row>
     <row r="253" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A253" s="0" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B253" s="0" t="s">
-        <v>137</v>
+        <v>353</v>
       </c>
       <c r="C253" s="0" t="s">
-        <v>137</v>
+        <v>353</v>
       </c>
     </row>
     <row r="254" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A254" s="0" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B254" s="0" t="s">
-        <v>150</v>
+        <v>58</v>
       </c>
       <c r="C254" s="0" t="s">
-        <v>150</v>
+        <v>58</v>
       </c>
     </row>
     <row r="255" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A255" s="0" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B255" s="0" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C255" s="0" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="256" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A256" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="B256" s="0" t="n">
-        <v>1</v>
+        <v>339</v>
+      </c>
+      <c r="B256" s="0" t="s">
+        <v>150</v>
       </c>
       <c r="C256" s="0" t="s">
-        <v>353</v>
+        <v>150</v>
       </c>
     </row>
     <row r="257" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A257" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="B257" s="0" t="n">
-        <v>2</v>
+        <v>339</v>
+      </c>
+      <c r="B257" s="0" t="s">
+        <v>135</v>
       </c>
       <c r="C257" s="0" t="s">
-        <v>354</v>
+        <v>135</v>
       </c>
     </row>
     <row r="258" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7191,10 +7185,10 @@
         <v>50</v>
       </c>
       <c r="B258" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C258" s="0" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="259" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7202,10 +7196,10 @@
         <v>50</v>
       </c>
       <c r="B259" s="0" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C259" s="0" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="260" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7213,10 +7207,10 @@
         <v>50</v>
       </c>
       <c r="B260" s="0" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C260" s="0" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="261" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7224,10 +7218,10 @@
         <v>50</v>
       </c>
       <c r="B261" s="0" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C261" s="0" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="262" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7235,10 +7229,10 @@
         <v>50</v>
       </c>
       <c r="B262" s="0" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C262" s="0" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="263" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7246,10 +7240,10 @@
         <v>50</v>
       </c>
       <c r="B263" s="0" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C263" s="0" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="264" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7257,10 +7251,10 @@
         <v>50</v>
       </c>
       <c r="B264" s="0" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C264" s="0" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="265" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7268,10 +7262,10 @@
         <v>50</v>
       </c>
       <c r="B265" s="0" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C265" s="0" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="266" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7279,10 +7273,10 @@
         <v>50</v>
       </c>
       <c r="B266" s="0" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C266" s="0" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="267" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7290,10 +7284,10 @@
         <v>50</v>
       </c>
       <c r="B267" s="0" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C267" s="0" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="268" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7301,10 +7295,10 @@
         <v>50</v>
       </c>
       <c r="B268" s="0" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C268" s="0" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="269" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7312,10 +7306,10 @@
         <v>50</v>
       </c>
       <c r="B269" s="0" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C269" s="0" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="270" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7323,10 +7317,10 @@
         <v>50</v>
       </c>
       <c r="B270" s="0" t="n">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C270" s="0" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="271" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7334,10 +7328,10 @@
         <v>50</v>
       </c>
       <c r="B271" s="0" t="n">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C271" s="0" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="272" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7345,10 +7339,10 @@
         <v>50</v>
       </c>
       <c r="B272" s="0" t="n">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C272" s="0" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="273" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7356,10 +7350,10 @@
         <v>50</v>
       </c>
       <c r="B273" s="0" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C273" s="0" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="274" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7367,10 +7361,10 @@
         <v>50</v>
       </c>
       <c r="B274" s="0" t="n">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C274" s="0" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="275" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7378,10 +7372,10 @@
         <v>50</v>
       </c>
       <c r="B275" s="0" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C275" s="0" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="276" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7389,10 +7383,10 @@
         <v>50</v>
       </c>
       <c r="B276" s="0" t="n">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C276" s="0" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="277" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7400,10 +7394,10 @@
         <v>50</v>
       </c>
       <c r="B277" s="0" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C277" s="0" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="278" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7411,10 +7405,10 @@
         <v>50</v>
       </c>
       <c r="B278" s="0" t="n">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C278" s="0" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="279" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7422,10 +7416,10 @@
         <v>50</v>
       </c>
       <c r="B279" s="0" t="n">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C279" s="0" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="280" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7433,10 +7427,10 @@
         <v>50</v>
       </c>
       <c r="B280" s="0" t="n">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C280" s="0" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="281" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7444,10 +7438,10 @@
         <v>50</v>
       </c>
       <c r="B281" s="0" t="n">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C281" s="0" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="282" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7455,10 +7449,10 @@
         <v>50</v>
       </c>
       <c r="B282" s="0" t="n">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C282" s="0" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="283" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7466,10 +7460,10 @@
         <v>50</v>
       </c>
       <c r="B283" s="0" t="n">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C283" s="0" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="284" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7477,10 +7471,10 @@
         <v>50</v>
       </c>
       <c r="B284" s="0" t="n">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C284" s="0" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="285" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7488,10 +7482,10 @@
         <v>50</v>
       </c>
       <c r="B285" s="0" t="n">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C285" s="0" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="286" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7499,32 +7493,32 @@
         <v>50</v>
       </c>
       <c r="B286" s="0" t="n">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C286" s="0" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="287" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A287" s="0" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="B287" s="0" t="n">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="C287" s="0" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="288" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A288" s="0" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="B288" s="0" t="n">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="C288" s="0" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="289" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7532,10 +7526,10 @@
         <v>64</v>
       </c>
       <c r="B289" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C289" s="0" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="290" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7543,10 +7537,10 @@
         <v>64</v>
       </c>
       <c r="B290" s="0" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C290" s="0" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="291" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7554,10 +7548,10 @@
         <v>64</v>
       </c>
       <c r="B291" s="0" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C291" s="0" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="292" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7565,10 +7559,10 @@
         <v>64</v>
       </c>
       <c r="B292" s="0" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C292" s="0" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="293" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7576,10 +7570,10 @@
         <v>64</v>
       </c>
       <c r="B293" s="0" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C293" s="0" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="294" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7587,10 +7581,10 @@
         <v>64</v>
       </c>
       <c r="B294" s="0" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C294" s="0" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="295" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7598,10 +7592,10 @@
         <v>64</v>
       </c>
       <c r="B295" s="0" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C295" s="0" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="296" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7609,10 +7603,10 @@
         <v>64</v>
       </c>
       <c r="B296" s="0" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C296" s="0" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="297" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7620,10 +7614,10 @@
         <v>64</v>
       </c>
       <c r="B297" s="0" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C297" s="0" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="298" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7631,32 +7625,32 @@
         <v>64</v>
       </c>
       <c r="B298" s="0" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C298" s="0" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="299" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A299" s="0" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="B299" s="0" t="n">
-        <v>2021</v>
+        <v>11</v>
       </c>
       <c r="C299" s="0" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="300" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A300" s="0" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="B300" s="0" t="n">
-        <v>2020</v>
+        <v>12</v>
       </c>
       <c r="C300" s="0" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="301" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7664,10 +7658,10 @@
         <v>71</v>
       </c>
       <c r="B301" s="0" t="n">
-        <v>2019</v>
+        <v>2021</v>
       </c>
       <c r="C301" s="0" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="302" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7675,10 +7669,10 @@
         <v>71</v>
       </c>
       <c r="B302" s="0" t="n">
-        <v>2018</v>
+        <v>2020</v>
       </c>
       <c r="C302" s="0" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="303" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7686,10 +7680,10 @@
         <v>71</v>
       </c>
       <c r="B303" s="0" t="n">
-        <v>2017</v>
+        <v>2019</v>
       </c>
       <c r="C303" s="0" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="304" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7697,10 +7691,10 @@
         <v>71</v>
       </c>
       <c r="B304" s="0" t="n">
-        <v>2016</v>
+        <v>2018</v>
       </c>
       <c r="C304" s="0" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="305" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7708,10 +7702,10 @@
         <v>71</v>
       </c>
       <c r="B305" s="0" t="n">
-        <v>2015</v>
+        <v>2017</v>
       </c>
       <c r="C305" s="0" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="306" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7719,10 +7713,10 @@
         <v>71</v>
       </c>
       <c r="B306" s="0" t="n">
-        <v>2014</v>
+        <v>2016</v>
       </c>
       <c r="C306" s="0" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="307" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7730,10 +7724,10 @@
         <v>71</v>
       </c>
       <c r="B307" s="0" t="n">
-        <v>2013</v>
+        <v>2015</v>
       </c>
       <c r="C307" s="0" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="308" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7741,10 +7735,10 @@
         <v>71</v>
       </c>
       <c r="B308" s="0" t="n">
-        <v>2012</v>
+        <v>2014</v>
       </c>
       <c r="C308" s="0" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="309" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7752,10 +7746,10 @@
         <v>71</v>
       </c>
       <c r="B309" s="0" t="n">
-        <v>2011</v>
+        <v>2013</v>
       </c>
       <c r="C309" s="0" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="310" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7763,10 +7757,10 @@
         <v>71</v>
       </c>
       <c r="B310" s="0" t="n">
-        <v>2010</v>
+        <v>2012</v>
       </c>
       <c r="C310" s="0" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="311" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7774,10 +7768,10 @@
         <v>71</v>
       </c>
       <c r="B311" s="0" t="n">
-        <v>2009</v>
+        <v>2011</v>
       </c>
       <c r="C311" s="0" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="312" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7785,10 +7779,10 @@
         <v>71</v>
       </c>
       <c r="B312" s="0" t="n">
-        <v>2008</v>
+        <v>2010</v>
       </c>
       <c r="C312" s="0" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="313" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7796,10 +7790,10 @@
         <v>71</v>
       </c>
       <c r="B313" s="0" t="n">
-        <v>2007</v>
+        <v>2009</v>
       </c>
       <c r="C313" s="0" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="314" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7807,10 +7801,10 @@
         <v>71</v>
       </c>
       <c r="B314" s="0" t="n">
-        <v>2006</v>
+        <v>2008</v>
       </c>
       <c r="C314" s="0" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="315" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7818,10 +7812,10 @@
         <v>71</v>
       </c>
       <c r="B315" s="0" t="n">
-        <v>2005</v>
+        <v>2007</v>
       </c>
       <c r="C315" s="0" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="316" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7829,10 +7823,10 @@
         <v>71</v>
       </c>
       <c r="B316" s="0" t="n">
-        <v>2004</v>
+        <v>2006</v>
       </c>
       <c r="C316" s="0" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="317" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7840,10 +7834,10 @@
         <v>71</v>
       </c>
       <c r="B317" s="0" t="n">
-        <v>2003</v>
+        <v>2005</v>
       </c>
       <c r="C317" s="0" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="318" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7851,10 +7845,10 @@
         <v>71</v>
       </c>
       <c r="B318" s="0" t="n">
-        <v>2002</v>
+        <v>2004</v>
       </c>
       <c r="C318" s="0" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="319" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7862,10 +7856,10 @@
         <v>71</v>
       </c>
       <c r="B319" s="0" t="n">
-        <v>2001</v>
+        <v>2003</v>
       </c>
       <c r="C319" s="0" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="320" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7873,10 +7867,10 @@
         <v>71</v>
       </c>
       <c r="B320" s="0" t="n">
-        <v>2000</v>
+        <v>2002</v>
       </c>
       <c r="C320" s="0" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="321" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7884,10 +7878,10 @@
         <v>71</v>
       </c>
       <c r="B321" s="0" t="n">
-        <v>1999</v>
+        <v>2001</v>
       </c>
       <c r="C321" s="0" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="322" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7895,10 +7889,10 @@
         <v>71</v>
       </c>
       <c r="B322" s="0" t="n">
-        <v>1998</v>
+        <v>2000</v>
       </c>
       <c r="C322" s="0" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="323" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7906,10 +7900,10 @@
         <v>71</v>
       </c>
       <c r="B323" s="0" t="n">
-        <v>1997</v>
+        <v>1999</v>
       </c>
       <c r="C323" s="0" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="324" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7917,10 +7911,10 @@
         <v>71</v>
       </c>
       <c r="B324" s="0" t="n">
-        <v>1996</v>
+        <v>1998</v>
       </c>
       <c r="C324" s="0" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="325" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7928,10 +7922,10 @@
         <v>71</v>
       </c>
       <c r="B325" s="0" t="n">
-        <v>1995</v>
+        <v>1997</v>
       </c>
       <c r="C325" s="0" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="326" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7939,10 +7933,10 @@
         <v>71</v>
       </c>
       <c r="B326" s="0" t="n">
-        <v>1994</v>
+        <v>1996</v>
       </c>
       <c r="C326" s="0" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="327" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7950,10 +7944,10 @@
         <v>71</v>
       </c>
       <c r="B327" s="0" t="n">
-        <v>1993</v>
+        <v>1995</v>
       </c>
       <c r="C327" s="0" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="328" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7961,10 +7955,10 @@
         <v>71</v>
       </c>
       <c r="B328" s="0" t="n">
-        <v>1992</v>
+        <v>1994</v>
       </c>
       <c r="C328" s="0" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="329" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7972,10 +7966,10 @@
         <v>71</v>
       </c>
       <c r="B329" s="0" t="n">
-        <v>1991</v>
+        <v>1993</v>
       </c>
       <c r="C329" s="0" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="330" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7983,10 +7977,10 @@
         <v>71</v>
       </c>
       <c r="B330" s="0" t="n">
-        <v>1990</v>
+        <v>1992</v>
       </c>
       <c r="C330" s="0" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="331" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7994,10 +7988,10 @@
         <v>71</v>
       </c>
       <c r="B331" s="0" t="n">
-        <v>1989</v>
+        <v>1991</v>
       </c>
       <c r="C331" s="0" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="332" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8005,10 +7999,10 @@
         <v>71</v>
       </c>
       <c r="B332" s="0" t="n">
-        <v>1988</v>
+        <v>1990</v>
       </c>
       <c r="C332" s="0" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="333" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8016,10 +8010,10 @@
         <v>71</v>
       </c>
       <c r="B333" s="0" t="n">
-        <v>1987</v>
+        <v>1989</v>
       </c>
       <c r="C333" s="0" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="334" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8027,10 +8021,10 @@
         <v>71</v>
       </c>
       <c r="B334" s="0" t="n">
-        <v>1986</v>
+        <v>1988</v>
       </c>
       <c r="C334" s="0" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="335" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8038,10 +8032,10 @@
         <v>71</v>
       </c>
       <c r="B335" s="0" t="n">
-        <v>1985</v>
+        <v>1987</v>
       </c>
       <c r="C335" s="0" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="336" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8049,10 +8043,10 @@
         <v>71</v>
       </c>
       <c r="B336" s="0" t="n">
-        <v>1984</v>
+        <v>1986</v>
       </c>
       <c r="C336" s="0" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="337" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8060,10 +8054,10 @@
         <v>71</v>
       </c>
       <c r="B337" s="0" t="n">
-        <v>1983</v>
+        <v>1985</v>
       </c>
       <c r="C337" s="0" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="338" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8071,10 +8065,10 @@
         <v>71</v>
       </c>
       <c r="B338" s="0" t="n">
-        <v>1982</v>
+        <v>1984</v>
       </c>
       <c r="C338" s="0" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="339" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8082,10 +8076,10 @@
         <v>71</v>
       </c>
       <c r="B339" s="0" t="n">
-        <v>1981</v>
+        <v>1983</v>
       </c>
       <c r="C339" s="0" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="340" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8093,10 +8087,10 @@
         <v>71</v>
       </c>
       <c r="B340" s="0" t="n">
-        <v>1980</v>
+        <v>1982</v>
       </c>
       <c r="C340" s="0" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="341" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8104,10 +8098,10 @@
         <v>71</v>
       </c>
       <c r="B341" s="0" t="n">
-        <v>1979</v>
+        <v>1981</v>
       </c>
       <c r="C341" s="0" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="342" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8115,10 +8109,10 @@
         <v>71</v>
       </c>
       <c r="B342" s="0" t="n">
-        <v>1978</v>
+        <v>1980</v>
       </c>
       <c r="C342" s="0" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="343" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8126,10 +8120,10 @@
         <v>71</v>
       </c>
       <c r="B343" s="0" t="n">
-        <v>1977</v>
+        <v>1979</v>
       </c>
       <c r="C343" s="0" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="344" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8137,10 +8131,10 @@
         <v>71</v>
       </c>
       <c r="B344" s="0" t="n">
-        <v>1976</v>
+        <v>1978</v>
       </c>
       <c r="C344" s="0" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="345" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8148,10 +8142,10 @@
         <v>71</v>
       </c>
       <c r="B345" s="0" t="n">
-        <v>1975</v>
+        <v>1977</v>
       </c>
       <c r="C345" s="0" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="346" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8159,10 +8153,10 @@
         <v>71</v>
       </c>
       <c r="B346" s="0" t="n">
-        <v>1974</v>
+        <v>1976</v>
       </c>
       <c r="C346" s="0" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="347" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8170,10 +8164,10 @@
         <v>71</v>
       </c>
       <c r="B347" s="0" t="n">
-        <v>1973</v>
+        <v>1975</v>
       </c>
       <c r="C347" s="0" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="348" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8181,10 +8175,10 @@
         <v>71</v>
       </c>
       <c r="B348" s="0" t="n">
-        <v>1972</v>
+        <v>1974</v>
       </c>
       <c r="C348" s="0" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="349" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8192,10 +8186,10 @@
         <v>71</v>
       </c>
       <c r="B349" s="0" t="n">
-        <v>1971</v>
+        <v>1973</v>
       </c>
       <c r="C349" s="0" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="350" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8203,10 +8197,10 @@
         <v>71</v>
       </c>
       <c r="B350" s="0" t="n">
-        <v>1970</v>
+        <v>1972</v>
       </c>
       <c r="C350" s="0" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="351" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8214,10 +8208,10 @@
         <v>71</v>
       </c>
       <c r="B351" s="0" t="n">
-        <v>1969</v>
+        <v>1971</v>
       </c>
       <c r="C351" s="0" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="352" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8225,10 +8219,10 @@
         <v>71</v>
       </c>
       <c r="B352" s="0" t="n">
-        <v>1968</v>
+        <v>1970</v>
       </c>
       <c r="C352" s="0" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="353" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8236,10 +8230,10 @@
         <v>71</v>
       </c>
       <c r="B353" s="0" t="n">
-        <v>1967</v>
+        <v>1969</v>
       </c>
       <c r="C353" s="0" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="354" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8247,10 +8241,10 @@
         <v>71</v>
       </c>
       <c r="B354" s="0" t="n">
-        <v>1966</v>
+        <v>1968</v>
       </c>
       <c r="C354" s="0" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="355" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8258,10 +8252,10 @@
         <v>71</v>
       </c>
       <c r="B355" s="0" t="n">
-        <v>1965</v>
+        <v>1967</v>
       </c>
       <c r="C355" s="0" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="356" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8269,10 +8263,10 @@
         <v>71</v>
       </c>
       <c r="B356" s="0" t="n">
-        <v>1964</v>
+        <v>1966</v>
       </c>
       <c r="C356" s="0" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="357" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8280,10 +8274,10 @@
         <v>71</v>
       </c>
       <c r="B357" s="0" t="n">
-        <v>1963</v>
+        <v>1965</v>
       </c>
       <c r="C357" s="0" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="358" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8291,10 +8285,10 @@
         <v>71</v>
       </c>
       <c r="B358" s="0" t="n">
-        <v>1962</v>
+        <v>1964</v>
       </c>
       <c r="C358" s="0" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="359" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8302,10 +8296,10 @@
         <v>71</v>
       </c>
       <c r="B359" s="0" t="n">
-        <v>1961</v>
+        <v>1963</v>
       </c>
       <c r="C359" s="0" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="360" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8313,10 +8307,10 @@
         <v>71</v>
       </c>
       <c r="B360" s="0" t="n">
-        <v>1960</v>
+        <v>1962</v>
       </c>
       <c r="C360" s="0" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="361" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8324,10 +8318,10 @@
         <v>71</v>
       </c>
       <c r="B361" s="0" t="n">
-        <v>1959</v>
+        <v>1961</v>
       </c>
       <c r="C361" s="0" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="362" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8335,10 +8329,10 @@
         <v>71</v>
       </c>
       <c r="B362" s="0" t="n">
-        <v>1958</v>
+        <v>1960</v>
       </c>
       <c r="C362" s="0" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="363" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8346,10 +8340,10 @@
         <v>71</v>
       </c>
       <c r="B363" s="0" t="n">
-        <v>1957</v>
+        <v>1959</v>
       </c>
       <c r="C363" s="0" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="364" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8357,10 +8351,10 @@
         <v>71</v>
       </c>
       <c r="B364" s="0" t="n">
-        <v>1956</v>
+        <v>1958</v>
       </c>
       <c r="C364" s="0" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="365" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8368,10 +8362,10 @@
         <v>71</v>
       </c>
       <c r="B365" s="0" t="n">
-        <v>1955</v>
+        <v>1957</v>
       </c>
       <c r="C365" s="0" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="366" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8379,10 +8373,10 @@
         <v>71</v>
       </c>
       <c r="B366" s="0" t="n">
-        <v>1954</v>
+        <v>1956</v>
       </c>
       <c r="C366" s="0" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="367" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8390,10 +8384,10 @@
         <v>71</v>
       </c>
       <c r="B367" s="0" t="n">
-        <v>1953</v>
+        <v>1955</v>
       </c>
       <c r="C367" s="0" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="368" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8401,10 +8395,10 @@
         <v>71</v>
       </c>
       <c r="B368" s="0" t="n">
-        <v>1952</v>
+        <v>1954</v>
       </c>
       <c r="C368" s="0" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="369" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8412,10 +8406,10 @@
         <v>71</v>
       </c>
       <c r="B369" s="0" t="n">
-        <v>1951</v>
+        <v>1953</v>
       </c>
       <c r="C369" s="0" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="370" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8423,10 +8417,10 @@
         <v>71</v>
       </c>
       <c r="B370" s="0" t="n">
-        <v>1950</v>
+        <v>1952</v>
       </c>
       <c r="C370" s="0" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="371" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8434,10 +8428,10 @@
         <v>71</v>
       </c>
       <c r="B371" s="0" t="n">
-        <v>1949</v>
+        <v>1951</v>
       </c>
       <c r="C371" s="0" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="372" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8445,10 +8439,10 @@
         <v>71</v>
       </c>
       <c r="B372" s="0" t="n">
-        <v>1948</v>
+        <v>1950</v>
       </c>
       <c r="C372" s="0" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="373" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8456,10 +8450,10 @@
         <v>71</v>
       </c>
       <c r="B373" s="0" t="n">
-        <v>1947</v>
+        <v>1949</v>
       </c>
       <c r="C373" s="0" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="374" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8467,10 +8461,10 @@
         <v>71</v>
       </c>
       <c r="B374" s="0" t="n">
-        <v>1946</v>
+        <v>1948</v>
       </c>
       <c r="C374" s="0" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="375" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8478,10 +8472,10 @@
         <v>71</v>
       </c>
       <c r="B375" s="0" t="n">
-        <v>1945</v>
+        <v>1947</v>
       </c>
       <c r="C375" s="0" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="376" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8489,10 +8483,10 @@
         <v>71</v>
       </c>
       <c r="B376" s="0" t="n">
-        <v>1944</v>
+        <v>1946</v>
       </c>
       <c r="C376" s="0" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="377" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8500,10 +8494,10 @@
         <v>71</v>
       </c>
       <c r="B377" s="0" t="n">
-        <v>1943</v>
+        <v>1945</v>
       </c>
       <c r="C377" s="0" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="378" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8511,10 +8505,10 @@
         <v>71</v>
       </c>
       <c r="B378" s="0" t="n">
-        <v>1942</v>
+        <v>1944</v>
       </c>
       <c r="C378" s="0" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="379" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8522,10 +8516,10 @@
         <v>71</v>
       </c>
       <c r="B379" s="0" t="n">
-        <v>1941</v>
+        <v>1943</v>
       </c>
       <c r="C379" s="0" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="380" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8533,10 +8527,10 @@
         <v>71</v>
       </c>
       <c r="B380" s="0" t="n">
-        <v>1940</v>
+        <v>1942</v>
       </c>
       <c r="C380" s="0" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="381" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8544,10 +8538,10 @@
         <v>71</v>
       </c>
       <c r="B381" s="0" t="n">
-        <v>1939</v>
+        <v>1941</v>
       </c>
       <c r="C381" s="0" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="382" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8555,10 +8549,10 @@
         <v>71</v>
       </c>
       <c r="B382" s="0" t="n">
-        <v>1938</v>
+        <v>1940</v>
       </c>
       <c r="C382" s="0" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="383" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8566,10 +8560,10 @@
         <v>71</v>
       </c>
       <c r="B383" s="0" t="n">
-        <v>1937</v>
+        <v>1939</v>
       </c>
       <c r="C383" s="0" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="384" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8577,10 +8571,10 @@
         <v>71</v>
       </c>
       <c r="B384" s="0" t="n">
-        <v>1936</v>
+        <v>1938</v>
       </c>
       <c r="C384" s="0" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="385" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8588,10 +8582,10 @@
         <v>71</v>
       </c>
       <c r="B385" s="0" t="n">
-        <v>1935</v>
+        <v>1937</v>
       </c>
       <c r="C385" s="0" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="386" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8599,10 +8593,10 @@
         <v>71</v>
       </c>
       <c r="B386" s="0" t="n">
-        <v>1934</v>
+        <v>1936</v>
       </c>
       <c r="C386" s="0" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="387" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8610,10 +8604,10 @@
         <v>71</v>
       </c>
       <c r="B387" s="0" t="n">
-        <v>1933</v>
+        <v>1935</v>
       </c>
       <c r="C387" s="0" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="388" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8621,10 +8615,10 @@
         <v>71</v>
       </c>
       <c r="B388" s="0" t="n">
-        <v>1932</v>
+        <v>1934</v>
       </c>
       <c r="C388" s="0" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="389" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8632,10 +8626,10 @@
         <v>71</v>
       </c>
       <c r="B389" s="0" t="n">
-        <v>1931</v>
+        <v>1933</v>
       </c>
       <c r="C389" s="0" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="390" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8643,10 +8637,10 @@
         <v>71</v>
       </c>
       <c r="B390" s="0" t="n">
-        <v>1930</v>
+        <v>1932</v>
       </c>
       <c r="C390" s="0" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="391" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8654,10 +8648,10 @@
         <v>71</v>
       </c>
       <c r="B391" s="0" t="n">
-        <v>1929</v>
+        <v>1931</v>
       </c>
       <c r="C391" s="0" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="392" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8665,10 +8659,10 @@
         <v>71</v>
       </c>
       <c r="B392" s="0" t="n">
-        <v>1928</v>
+        <v>1930</v>
       </c>
       <c r="C392" s="0" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="393" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8676,10 +8670,10 @@
         <v>71</v>
       </c>
       <c r="B393" s="0" t="n">
-        <v>1927</v>
+        <v>1929</v>
       </c>
       <c r="C393" s="0" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="394" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8687,10 +8681,10 @@
         <v>71</v>
       </c>
       <c r="B394" s="0" t="n">
-        <v>1926</v>
+        <v>1928</v>
       </c>
       <c r="C394" s="0" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="395" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8698,10 +8692,10 @@
         <v>71</v>
       </c>
       <c r="B395" s="0" t="n">
-        <v>1925</v>
+        <v>1927</v>
       </c>
       <c r="C395" s="0" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="396" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8709,10 +8703,10 @@
         <v>71</v>
       </c>
       <c r="B396" s="0" t="n">
-        <v>1924</v>
+        <v>1926</v>
       </c>
       <c r="C396" s="0" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="397" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8720,10 +8714,10 @@
         <v>71</v>
       </c>
       <c r="B397" s="0" t="n">
-        <v>1923</v>
+        <v>1925</v>
       </c>
       <c r="C397" s="0" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="398" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8731,10 +8725,10 @@
         <v>71</v>
       </c>
       <c r="B398" s="0" t="n">
-        <v>1922</v>
+        <v>1924</v>
       </c>
       <c r="C398" s="0" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="399" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8742,10 +8736,10 @@
         <v>71</v>
       </c>
       <c r="B399" s="0" t="n">
-        <v>1921</v>
+        <v>1923</v>
       </c>
       <c r="C399" s="0" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="400" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8753,10 +8747,32 @@
         <v>71</v>
       </c>
       <c r="B400" s="0" t="n">
+        <v>1922</v>
+      </c>
+      <c r="C400" s="0" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="401" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A401" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="B401" s="0" t="n">
+        <v>1921</v>
+      </c>
+      <c r="C401" s="0" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="402" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A402" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="B402" s="0" t="n">
         <v>1920</v>
       </c>
-      <c r="C400" s="0" t="s">
-        <v>497</v>
+      <c r="C402" s="0" t="s">
+        <v>498</v>
       </c>
     </row>
   </sheetData>
@@ -8775,10 +8791,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H763"/>
+  <dimension ref="A1:H1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.25" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8796,7 +8812,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>7</v>
@@ -8805,77 +8821,77 @@
         <v>1</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="D2" s="8"/>
       <c r="F2" s="7"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="8" t="s">
+        <v>508</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>507</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>506</v>
       </c>
       <c r="D3" s="8"/>
       <c r="F3" s="7"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="8" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="D4" s="8"/>
       <c r="F4" s="7"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="8" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="F5" s="7" t="n">
         <v>1</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="8" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>78</v>
@@ -8885,7 +8901,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="8" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>78</v>
@@ -8895,7 +8911,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="8" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>78</v>
@@ -8905,7 +8921,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="8" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>78</v>
@@ -8915,7 +8931,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="8" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>78</v>
@@ -8925,7 +8941,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="8" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>78</v>
@@ -8935,7 +8951,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="8" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>78</v>
@@ -8945,7 +8961,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="B13" s="9" t="s">
         <v>7</v>
@@ -9096,10 +9112,10 @@
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="C26" s="10" t="s">
         <v>26</v>
@@ -9112,271 +9128,271 @@
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="10" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="D27" s="10"/>
       <c r="F27" s="7"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="10" t="s">
-        <v>524</v>
+        <v>139</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>78</v>
+        <v>26</v>
       </c>
       <c r="D28" s="10"/>
+      <c r="E28" s="0" t="s">
+        <v>139</v>
+      </c>
       <c r="F28" s="7"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="10" t="s">
+      <c r="A29" s="0" t="s">
         <v>525</v>
       </c>
-      <c r="C29" s="10" t="s">
+      <c r="B29" s="11" t="s">
+        <v>260</v>
+      </c>
+      <c r="C29" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="D29" s="10"/>
+      <c r="D29" s="11"/>
       <c r="E29" s="0" t="s">
-        <v>209</v>
+        <v>260</v>
       </c>
       <c r="F29" s="7"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="10" t="s">
+      <c r="B30" s="11" t="s">
         <v>526</v>
       </c>
-      <c r="C30" s="10" t="s">
+      <c r="C30" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="D30" s="11"/>
+      <c r="F30" s="7"/>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="11" t="s">
+        <v>527</v>
+      </c>
+      <c r="C31" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="D30" s="10"/>
-      <c r="E30" s="0" t="s">
+      <c r="D31" s="11"/>
+      <c r="E31" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="F30" s="7"/>
-    </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="10" t="s">
-        <v>139</v>
-      </c>
-      <c r="C31" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D31" s="10"/>
-      <c r="E31" s="0" t="s">
-        <v>139</v>
-      </c>
       <c r="F31" s="7"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
-        <v>527</v>
-      </c>
       <c r="B32" s="11" t="s">
-        <v>260</v>
+        <v>528</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>26</v>
+        <v>103</v>
       </c>
       <c r="D32" s="11"/>
-      <c r="E32" s="0" t="s">
-        <v>260</v>
-      </c>
       <c r="F32" s="7"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="11" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>103</v>
+        <v>78</v>
       </c>
       <c r="D33" s="11"/>
       <c r="F33" s="7"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="11" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>57</v>
+        <v>26</v>
       </c>
       <c r="D34" s="11"/>
       <c r="E34" s="0" t="s">
-        <v>58</v>
+        <v>110</v>
       </c>
       <c r="F34" s="7"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="11" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="C35" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D35" s="11"/>
+      <c r="E35" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="F35" s="7"/>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>532</v>
+      </c>
+      <c r="B36" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D36" s="12"/>
+      <c r="E36" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="F36" s="7"/>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="C37" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="D35" s="11"/>
-      <c r="F35" s="7"/>
-    </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="11" t="s">
-        <v>531</v>
-      </c>
-      <c r="C36" s="11" t="s">
+      <c r="D37" s="12"/>
+      <c r="F37" s="7"/>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="C38" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="D36" s="11"/>
-      <c r="F36" s="7"/>
-    </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="11" t="s">
-        <v>532</v>
-      </c>
-      <c r="C37" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="D37" s="11"/>
-      <c r="E37" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="F37" s="7"/>
-    </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="11" t="s">
-        <v>533</v>
-      </c>
-      <c r="C38" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="D38" s="11"/>
-      <c r="E38" s="0" t="s">
-        <v>112</v>
-      </c>
+      <c r="D38" s="12"/>
       <c r="F38" s="7"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
-        <v>534</v>
-      </c>
       <c r="B39" s="12" t="s">
-        <v>28</v>
+        <v>111</v>
       </c>
       <c r="C39" s="12" t="s">
         <v>26</v>
       </c>
       <c r="D39" s="12"/>
       <c r="E39" s="0" t="s">
-        <v>27</v>
+        <v>110</v>
       </c>
       <c r="F39" s="7"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="12" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>103</v>
+        <v>26</v>
       </c>
       <c r="D40" s="12"/>
+      <c r="E40" s="0" t="s">
+        <v>112</v>
+      </c>
       <c r="F40" s="7"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="12" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>78</v>
+        <v>26</v>
       </c>
       <c r="D41" s="12"/>
+      <c r="E41" s="0" t="s">
+        <v>116</v>
+      </c>
       <c r="F41" s="7"/>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="12" t="s">
-        <v>111</v>
+        <v>124</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>26</v>
+        <v>57</v>
       </c>
       <c r="D42" s="12"/>
       <c r="E42" s="0" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="F42" s="7"/>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="C43" s="12" t="s">
+      <c r="A43" s="0" t="s">
+        <v>533</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>534</v>
+      </c>
+      <c r="C43" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D43" s="12"/>
+      <c r="D43" s="9"/>
       <c r="E43" s="0" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="F43" s="7"/>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="C44" s="12" t="s">
+      <c r="B44" s="9" t="s">
+        <v>535</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="D44" s="9"/>
+      <c r="E44" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="F44" s="7"/>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>536</v>
+      </c>
+      <c r="B45" s="13" t="s">
+        <v>537</v>
+      </c>
+      <c r="C45" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="D45" s="13"/>
+      <c r="F45" s="7"/>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B46" s="13" t="s">
+        <v>538</v>
+      </c>
+      <c r="C46" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="D46" s="13"/>
+      <c r="E46" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="F46" s="7"/>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B47" s="13" t="s">
+        <v>539</v>
+      </c>
+      <c r="C47" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="D44" s="12"/>
-      <c r="E44" s="0" t="s">
+      <c r="D47" s="13"/>
+      <c r="E47" s="0" t="s">
         <v>116</v>
       </c>
-      <c r="F44" s="7"/>
-    </row>
-    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="12" t="s">
-        <v>124</v>
-      </c>
-      <c r="C45" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="D45" s="12"/>
-      <c r="E45" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="F45" s="7"/>
-    </row>
-    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
-        <v>535</v>
-      </c>
-      <c r="B46" s="9" t="s">
-        <v>536</v>
-      </c>
-      <c r="C46" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="D46" s="9"/>
-      <c r="E46" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="F46" s="7"/>
-    </row>
-    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="9" t="s">
-        <v>537</v>
-      </c>
-      <c r="C47" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="D47" s="9"/>
-      <c r="E47" s="0" t="s">
-        <v>123</v>
-      </c>
       <c r="F47" s="7"/>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
-        <v>538</v>
-      </c>
       <c r="B48" s="13" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="C48" s="13" t="s">
         <v>78</v>
@@ -9386,108 +9402,108 @@
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="13" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="C49" s="13" t="s">
         <v>57</v>
       </c>
       <c r="D49" s="13"/>
       <c r="E49" s="0" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F49" s="7"/>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="13" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="C50" s="13" t="s">
-        <v>26</v>
+        <v>57</v>
       </c>
       <c r="D50" s="13"/>
       <c r="E50" s="0" t="s">
-        <v>116</v>
+        <v>169</v>
       </c>
       <c r="F50" s="7"/>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="13" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="C51" s="13" t="s">
-        <v>78</v>
+        <v>33</v>
       </c>
       <c r="D51" s="13"/>
       <c r="F51" s="7"/>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="13" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="C52" s="13" t="s">
-        <v>57</v>
+        <v>26</v>
       </c>
       <c r="D52" s="13"/>
       <c r="E52" s="0" t="s">
-        <v>58</v>
+        <v>174</v>
       </c>
       <c r="F52" s="7"/>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B53" s="13" t="s">
-        <v>544</v>
-      </c>
-      <c r="C53" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="D53" s="13"/>
+      <c r="A53" s="0" t="s">
+        <v>545</v>
+      </c>
+      <c r="B53" s="14" t="s">
+        <v>546</v>
+      </c>
+      <c r="C53" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D53" s="14"/>
       <c r="E53" s="0" t="s">
-        <v>169</v>
+        <v>133</v>
       </c>
       <c r="F53" s="7"/>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B54" s="13" t="s">
-        <v>545</v>
-      </c>
-      <c r="C54" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="D54" s="13"/>
+      <c r="B54" s="14" t="s">
+        <v>547</v>
+      </c>
+      <c r="C54" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D54" s="14"/>
+      <c r="E54" s="0" t="s">
+        <v>133</v>
+      </c>
       <c r="F54" s="7"/>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B55" s="13" t="s">
-        <v>546</v>
-      </c>
-      <c r="C55" s="13" t="s">
+      <c r="B55" s="14" t="s">
+        <v>548</v>
+      </c>
+      <c r="C55" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D55" s="13"/>
+      <c r="D55" s="14"/>
       <c r="E55" s="0" t="s">
-        <v>174</v>
+        <v>133</v>
       </c>
       <c r="F55" s="7"/>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0" t="s">
-        <v>547</v>
-      </c>
       <c r="B56" s="14" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="C56" s="14" t="s">
-        <v>26</v>
+        <v>550</v>
       </c>
       <c r="D56" s="14"/>
-      <c r="E56" s="0" t="s">
-        <v>133</v>
-      </c>
       <c r="F56" s="7"/>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="14" t="s">
-        <v>549</v>
+        <v>551</v>
       </c>
       <c r="C57" s="14" t="s">
         <v>26</v>
@@ -9500,58 +9516,61 @@
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="14" t="s">
+        <v>552</v>
+      </c>
+      <c r="C58" s="14" t="s">
         <v>550</v>
       </c>
-      <c r="C58" s="14" t="s">
-        <v>26</v>
-      </c>
       <c r="D58" s="14"/>
-      <c r="E58" s="0" t="s">
-        <v>133</v>
-      </c>
       <c r="F58" s="7"/>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="14" t="s">
-        <v>551</v>
+        <v>553</v>
       </c>
       <c r="C59" s="14" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="D59" s="14"/>
       <c r="F59" s="7"/>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="14" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="C60" s="14" t="s">
         <v>26</v>
       </c>
       <c r="D60" s="14"/>
       <c r="E60" s="0" t="s">
-        <v>133</v>
+        <v>290</v>
       </c>
       <c r="F60" s="7"/>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B61" s="14" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="C61" s="14" t="s">
-        <v>552</v>
+        <v>26</v>
       </c>
       <c r="D61" s="14"/>
+      <c r="E61" s="0" t="s">
+        <v>295</v>
+      </c>
       <c r="F61" s="7"/>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="14" t="s">
-        <v>555</v>
+        <v>228</v>
       </c>
       <c r="C62" s="14" t="s">
-        <v>552</v>
+        <v>26</v>
       </c>
       <c r="D62" s="14"/>
+      <c r="E62" s="0" t="s">
+        <v>228</v>
+      </c>
       <c r="F62" s="7"/>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9559,82 +9578,79 @@
         <v>556</v>
       </c>
       <c r="C63" s="14" t="s">
-        <v>26</v>
+        <v>557</v>
       </c>
       <c r="D63" s="14"/>
       <c r="E63" s="0" t="s">
-        <v>290</v>
+        <v>558</v>
       </c>
       <c r="F63" s="7"/>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B64" s="14" t="s">
-        <v>557</v>
+        <v>559</v>
       </c>
       <c r="C64" s="14" t="s">
-        <v>26</v>
+        <v>57</v>
       </c>
       <c r="D64" s="14"/>
       <c r="E64" s="0" t="s">
-        <v>295</v>
+        <v>339</v>
       </c>
       <c r="F64" s="7"/>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B65" s="14" t="s">
-        <v>228</v>
+        <v>560</v>
       </c>
       <c r="C65" s="14" t="s">
-        <v>26</v>
+        <v>57</v>
       </c>
       <c r="D65" s="14"/>
       <c r="E65" s="0" t="s">
-        <v>228</v>
+        <v>183</v>
       </c>
       <c r="F65" s="7"/>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B66" s="14" t="s">
-        <v>558</v>
+        <v>561</v>
       </c>
       <c r="C66" s="14" t="s">
-        <v>559</v>
+        <v>33</v>
       </c>
       <c r="D66" s="14"/>
-      <c r="E66" s="0" t="s">
-        <v>560</v>
-      </c>
       <c r="F66" s="7"/>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B67" s="14" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="C67" s="14" t="s">
-        <v>57</v>
+        <v>26</v>
       </c>
       <c r="D67" s="14"/>
       <c r="E67" s="0" t="s">
-        <v>338</v>
+        <v>116</v>
       </c>
       <c r="F67" s="7"/>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B68" s="14" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="C68" s="14" t="s">
         <v>57</v>
       </c>
       <c r="D68" s="14"/>
       <c r="E68" s="0" t="s">
-        <v>183</v>
+        <v>277</v>
       </c>
       <c r="F68" s="7"/>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B69" s="14" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="C69" s="14" t="s">
         <v>33</v>
@@ -9644,56 +9660,56 @@
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B70" s="14" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="C70" s="14" t="s">
-        <v>26</v>
+        <v>57</v>
       </c>
       <c r="D70" s="14"/>
       <c r="E70" s="0" t="s">
-        <v>116</v>
+        <v>282</v>
       </c>
       <c r="F70" s="7"/>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B71" s="14" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="C71" s="14" t="s">
-        <v>57</v>
+        <v>33</v>
       </c>
       <c r="D71" s="14"/>
-      <c r="E71" s="0" t="s">
-        <v>277</v>
-      </c>
       <c r="F71" s="7"/>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B72" s="14" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="C72" s="14" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="D72" s="14"/>
+      <c r="E72" s="0" t="s">
+        <v>133</v>
+      </c>
       <c r="F72" s="7"/>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B73" s="14" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="C73" s="14" t="s">
         <v>57</v>
       </c>
       <c r="D73" s="14"/>
       <c r="E73" s="0" t="s">
-        <v>282</v>
+        <v>214</v>
       </c>
       <c r="F73" s="7"/>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B74" s="14" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="C74" s="14" t="s">
         <v>33</v>
@@ -9703,147 +9719,150 @@
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B75" s="14" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="C75" s="14" t="s">
         <v>26</v>
       </c>
       <c r="D75" s="14"/>
       <c r="E75" s="0" t="s">
-        <v>133</v>
+        <v>116</v>
       </c>
       <c r="F75" s="7"/>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B76" s="14" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="C76" s="14" t="s">
-        <v>57</v>
+        <v>26</v>
       </c>
       <c r="D76" s="14"/>
       <c r="E76" s="0" t="s">
-        <v>214</v>
+        <v>256</v>
       </c>
       <c r="F76" s="7"/>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B77" s="14" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="C77" s="14" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="D77" s="14"/>
+      <c r="E77" s="0" t="s">
+        <v>116</v>
+      </c>
       <c r="F77" s="7"/>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B78" s="14" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="C78" s="14" t="s">
         <v>26</v>
       </c>
       <c r="D78" s="14"/>
       <c r="E78" s="0" t="s">
-        <v>116</v>
+        <v>251</v>
       </c>
       <c r="F78" s="7"/>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B79" s="14" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="C79" s="14" t="s">
-        <v>26</v>
+        <v>57</v>
       </c>
       <c r="D79" s="14"/>
       <c r="E79" s="0" t="s">
-        <v>256</v>
+        <v>197</v>
       </c>
       <c r="F79" s="7"/>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B80" s="14" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="C80" s="14" t="s">
-        <v>26</v>
+        <v>57</v>
       </c>
       <c r="D80" s="14"/>
       <c r="E80" s="0" t="s">
-        <v>116</v>
+        <v>244</v>
       </c>
       <c r="F80" s="7"/>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B81" s="14" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="C81" s="14" t="s">
         <v>26</v>
       </c>
       <c r="D81" s="14"/>
       <c r="E81" s="0" t="s">
-        <v>251</v>
+        <v>136</v>
       </c>
       <c r="F81" s="7"/>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B82" s="14" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="C82" s="14" t="s">
-        <v>57</v>
+        <v>26</v>
       </c>
       <c r="D82" s="14"/>
       <c r="E82" s="0" t="s">
-        <v>197</v>
+        <v>136</v>
       </c>
       <c r="F82" s="7"/>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B83" s="14" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="C83" s="14" t="s">
-        <v>57</v>
+        <v>26</v>
       </c>
       <c r="D83" s="14"/>
       <c r="E83" s="0" t="s">
-        <v>244</v>
+        <v>136</v>
       </c>
       <c r="F83" s="7"/>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B84" s="14" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="C84" s="14" t="s">
         <v>26</v>
       </c>
       <c r="D84" s="14"/>
       <c r="E84" s="0" t="s">
-        <v>136</v>
+        <v>247</v>
       </c>
       <c r="F84" s="7"/>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B85" s="14" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="C85" s="14" t="s">
         <v>26</v>
       </c>
       <c r="D85" s="14"/>
       <c r="E85" s="0" t="s">
-        <v>136</v>
+        <v>179</v>
       </c>
       <c r="F85" s="7"/>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B86" s="14" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="C86" s="14" t="s">
         <v>26</v>
@@ -9856,66 +9875,63 @@
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B87" s="14" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="C87" s="14" t="s">
         <v>26</v>
       </c>
       <c r="D87" s="14"/>
       <c r="E87" s="0" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="F87" s="7"/>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B88" s="14" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="C88" s="14" t="s">
         <v>26</v>
       </c>
       <c r="D88" s="14"/>
       <c r="E88" s="0" t="s">
-        <v>179</v>
+        <v>116</v>
       </c>
       <c r="F88" s="7"/>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B89" s="14" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="C89" s="14" t="s">
-        <v>26</v>
+        <v>78</v>
       </c>
       <c r="D89" s="14"/>
-      <c r="E89" s="0" t="s">
-        <v>136</v>
-      </c>
       <c r="F89" s="7"/>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B90" s="14" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="C90" s="14" t="s">
         <v>26</v>
       </c>
       <c r="D90" s="14"/>
       <c r="E90" s="0" t="s">
-        <v>239</v>
+        <v>58</v>
       </c>
       <c r="F90" s="7"/>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B91" s="14" t="s">
-        <v>585</v>
+        <v>326</v>
       </c>
       <c r="C91" s="14" t="s">
         <v>26</v>
       </c>
       <c r="D91" s="14"/>
       <c r="E91" s="0" t="s">
-        <v>116</v>
+        <v>326</v>
       </c>
       <c r="F91" s="7"/>
     </row>
@@ -9924,9 +9940,12 @@
         <v>586</v>
       </c>
       <c r="C92" s="14" t="s">
-        <v>78</v>
+        <v>26</v>
       </c>
       <c r="D92" s="14"/>
+      <c r="E92" s="0" t="s">
+        <v>320</v>
+      </c>
       <c r="F92" s="7"/>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9934,76 +9953,76 @@
         <v>587</v>
       </c>
       <c r="C93" s="14" t="s">
-        <v>26</v>
+        <v>57</v>
       </c>
       <c r="D93" s="14"/>
       <c r="E93" s="0" t="s">
-        <v>58</v>
+        <v>151</v>
       </c>
       <c r="F93" s="7"/>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B94" s="14" t="s">
-        <v>325</v>
+        <v>588</v>
       </c>
       <c r="C94" s="14" t="s">
         <v>26</v>
       </c>
       <c r="D94" s="14"/>
       <c r="E94" s="0" t="s">
-        <v>325</v>
+        <v>315</v>
       </c>
       <c r="F94" s="7"/>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B95" s="14" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="C95" s="14" t="s">
         <v>26</v>
       </c>
       <c r="D95" s="14"/>
       <c r="E95" s="0" t="s">
-        <v>319</v>
+        <v>327</v>
       </c>
       <c r="F95" s="7"/>
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B96" s="14" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="C96" s="14" t="s">
         <v>57</v>
       </c>
       <c r="D96" s="14"/>
       <c r="E96" s="0" t="s">
-        <v>151</v>
+        <v>163</v>
       </c>
       <c r="F96" s="7"/>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B97" s="14" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="C97" s="14" t="s">
         <v>26</v>
       </c>
       <c r="D97" s="14"/>
       <c r="E97" s="0" t="s">
-        <v>314</v>
+        <v>133</v>
       </c>
       <c r="F97" s="7"/>
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B98" s="14" t="s">
-        <v>591</v>
+        <v>328</v>
       </c>
       <c r="C98" s="14" t="s">
-        <v>26</v>
+        <v>57</v>
       </c>
       <c r="D98" s="14"/>
       <c r="E98" s="0" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="F98" s="7"/>
     </row>
@@ -10012,11 +10031,11 @@
         <v>592</v>
       </c>
       <c r="C99" s="14" t="s">
-        <v>57</v>
+        <v>26</v>
       </c>
       <c r="D99" s="14"/>
       <c r="E99" s="0" t="s">
-        <v>163</v>
+        <v>138</v>
       </c>
       <c r="F99" s="7"/>
     </row>
@@ -10025,48 +10044,18 @@
         <v>593</v>
       </c>
       <c r="C100" s="14" t="s">
-        <v>26</v>
+        <v>78</v>
       </c>
       <c r="D100" s="14"/>
-      <c r="E100" s="0" t="s">
-        <v>133</v>
-      </c>
       <c r="F100" s="7"/>
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B101" s="14" t="s">
-        <v>327</v>
-      </c>
-      <c r="C101" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="D101" s="14"/>
-      <c r="E101" s="0" t="s">
-        <v>327</v>
-      </c>
       <c r="F101" s="7"/>
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B102" s="14" t="s">
-        <v>594</v>
-      </c>
-      <c r="C102" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="D102" s="14"/>
-      <c r="E102" s="0" t="s">
-        <v>138</v>
-      </c>
       <c r="F102" s="7"/>
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B103" s="14" t="s">
-        <v>595</v>
-      </c>
-      <c r="C103" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="D103" s="14"/>
       <c r="F103" s="7"/>
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12040,15 +12029,9 @@
     <row r="760" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F760" s="7"/>
     </row>
-    <row r="761" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F761" s="7"/>
-    </row>
-    <row r="762" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F762" s="7"/>
-    </row>
-    <row r="763" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F763" s="7"/>
-    </row>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -12068,7 +12051,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.25" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12083,75 +12066,75 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="15" t="s">
+        <v>594</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>595</v>
+      </c>
+      <c r="C1" s="0" t="s">
         <v>596</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="D1" s="0" t="s">
         <v>597</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="E1" s="0" t="s">
         <v>598</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="F1" s="0" t="s">
         <v>599</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="G1" s="0" t="s">
         <v>600</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="H1" s="0" t="s">
         <v>601</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>602</v>
-      </c>
-      <c r="H1" s="0" t="s">
-        <v>603</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="15" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="C2" s="15"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="15" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="B3" s="7" t="n">
-        <v>20210221001</v>
+        <v>20210223001</v>
       </c>
       <c r="C3" s="15"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="15" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="C4" s="15"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="15" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="B5" s="15"/>
       <c r="C5" s="15" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="15" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>7</v>
@@ -12160,49 +12143,49 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>1</v>

</xml_diff>